<commit_message>
Fix the Excel shenanigans (:shipit:)
</commit_message>
<xml_diff>
--- a/src/test/resources/sample.xlsx
+++ b/src/test/resources/sample.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Date &amp; Time</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>Reversal</t>
+  </si>
+  <si>
+    <t>28/08/2017 07:08</t>
+  </si>
+  <si>
+    <t>28/08/2017 07:30</t>
+  </si>
+  <si>
+    <t>28/08/2017 07:33</t>
   </si>
 </sst>
 </file>
@@ -90,7 +99,14 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\£#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,28 +176,28 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -507,7 +523,7 @@
   <dimension ref="B2:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,8 +579,8 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="6">
-        <v>42975.291666666664</v>
+      <c r="B7" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -572,13 +588,13 @@
       <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="4" t="s">
@@ -595,8 +611,8 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="6">
-        <v>42975.3125</v>
+      <c r="B8" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -607,10 +623,10 @@
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -627,8 +643,8 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="6">
-        <v>42975.333333333336</v>
+      <c r="B9" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -639,10 +655,10 @@
       <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="4" t="s">

</xml_diff>